<commit_message>
Bug fix: Exotics on NFL Preseason
</commit_message>
<xml_diff>
--- a/DesktopC/bin/Debug/BASE.xlsx
+++ b/DesktopC/bin/Debug/BASE.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Volume</t>
   </si>
@@ -44,24 +44,15 @@
     <t>MLB ML</t>
   </si>
   <si>
-    <t>ML</t>
-  </si>
-  <si>
     <t>MLB SP</t>
   </si>
   <si>
-    <t>SPREAD</t>
-  </si>
-  <si>
     <t>MLB TOTAL</t>
   </si>
   <si>
     <t>SOCCER TOTAL</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>MLB 1H ML</t>
   </si>
   <si>
@@ -150,9 +141,6 @@
   </si>
   <si>
     <t>JULY 30TH</t>
-  </si>
-  <si>
-    <t>AUG 6TH</t>
   </si>
   <si>
     <t xml:space="preserve">NFL PRESEASON </t>
@@ -515,47 +503,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -934,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,15 +896,13 @@
     <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -967,9 +913,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
@@ -979,9 +923,7 @@
       <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="K1" s="1"/>
       <c r="L1" s="2" t="s">
         <v>0</v>
       </c>
@@ -994,7 +936,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1031,9 +973,7 @@
         <f>(H3/G3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>6</v>
-      </c>
+      <c r="K3" s="11"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
       <c r="N3" s="8" t="e">
@@ -1043,7 +983,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1059,9 +999,7 @@
         <f t="shared" ref="I4:I13" si="2">(H4/G4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4" s="11" t="s">
-        <v>8</v>
-      </c>
+      <c r="K4" s="11"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="8" t="e">
@@ -1071,7 +1009,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -1087,9 +1025,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="K5" s="11"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="8" t="e">
@@ -1099,7 +1035,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -1116,7 +1052,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L6" s="10">
         <f>SUM(L3:L5)</f>
@@ -1133,7 +1069,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1152,7 +1088,7 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -1171,7 +1107,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1187,9 +1123,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="K9" s="1"/>
       <c r="L9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1136,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1219,7 +1153,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
@@ -1227,7 +1161,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -1253,7 +1187,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -1263,7 +1197,7 @@
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="14"/>
@@ -1281,7 +1215,7 @@
     </row>
     <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -1291,7 +1225,7 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G13" s="16">
         <f>SUM(G3:G12)</f>
@@ -1315,7 +1249,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -1338,7 +1272,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1357,7 +1291,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -1366,9 +1300,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="2" t="s">
         <v>0</v>
       </c>
@@ -1388,7 +1320,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -1398,7 +1330,7 @@
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1413,7 +1345,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -1439,7 +1371,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -1465,7 +1397,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -1491,7 +1423,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -1517,7 +1449,7 @@
     </row>
     <row r="22" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="16">
         <f>SUM(B3:B21)</f>
@@ -1561,7 +1493,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
@@ -1572,7 +1504,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>0</v>
@@ -1592,7 +1524,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L24" s="10">
         <f>SUM(L11:L23)</f>
@@ -1609,7 +1541,7 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1625,7 +1557,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -1641,9 +1573,7 @@
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="K26" s="1"/>
       <c r="L26" s="2" t="s">
         <v>0</v>
       </c>
@@ -1656,7 +1586,7 @@
     </row>
     <row r="27" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B27" s="16">
         <f>SUM(B26)</f>
@@ -1672,7 +1602,7 @@
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -1681,7 +1611,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
@@ -1690,7 +1620,7 @@
     <row r="28" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="4"/>
       <c r="F28" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G28" s="16">
         <f>SUM(G18:G27)</f>
@@ -1714,7 +1644,7 @@
     </row>
     <row r="29" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>0</v>
@@ -1750,14 +1680,14 @@
     </row>
     <row r="31" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B31" s="28">
-        <f>(B22+G13+L6+B26+G28+L24)</f>
+        <f>(B22+G13+L6+B27+G28+L24+L41)</f>
         <v>0</v>
       </c>
       <c r="C31" s="28">
-        <f>(C22+C26+H28+H13+M6+M24)</f>
+        <f>(C22+C27+H28+H13+M6+M24+M41)</f>
         <v>0</v>
       </c>
       <c r="D31" s="29" t="e">
@@ -1847,7 +1777,7 @@
     </row>
     <row r="40" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K40" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L40" s="10">
         <v>0</v>
@@ -1862,7 +1792,7 @@
     </row>
     <row r="41" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K41" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L41" s="10">
         <f>SUM(L28:L40)</f>
@@ -1879,42 +1809,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C31:D31 C26:D27 H3:I13 H18:I28 M3:N6 C3:D22">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:N23">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24:N24">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M28:N40">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M41:N41">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
G8 House report update
</commit_message>
<xml_diff>
--- a/DesktopC/bin/Debug/BASE.xlsx
+++ b/DesktopC/bin/Debug/BASE.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents2017\desktop\ReportGameStats\DesktopC\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rtc-domain\FolderRedirection\luisma\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30600" windowHeight="6255"/>
   </bookViews>
   <sheets>
-    <sheet name="JUL 30TH" sheetId="7" r:id="rId1"/>
+    <sheet name="2017-08-26" sheetId="7" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>Volume</t>
   </si>
@@ -140,10 +140,64 @@
     <t>MLB</t>
   </si>
   <si>
-    <t>JULY 30TH</t>
-  </si>
-  <si>
     <t xml:space="preserve">NFL PRESEASON </t>
+  </si>
+  <si>
+    <t>GAME ML</t>
+  </si>
+  <si>
+    <t>FIRST HALF PS</t>
+  </si>
+  <si>
+    <t>SECOND HALF ML</t>
+  </si>
+  <si>
+    <t>SOC   ML</t>
+  </si>
+  <si>
+    <t>GAME PS</t>
+  </si>
+  <si>
+    <t>FIRST HALF Total</t>
+  </si>
+  <si>
+    <t>SECOND HALF PS</t>
+  </si>
+  <si>
+    <t>SOC   PS</t>
+  </si>
+  <si>
+    <t>GAME Total</t>
+  </si>
+  <si>
+    <t>SECOND HALF Total</t>
+  </si>
+  <si>
+    <t>SOC   Total</t>
+  </si>
+  <si>
+    <t>COLLEGE FB</t>
+  </si>
+  <si>
+    <t>NFL</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>NHL PRESEASON</t>
+  </si>
+  <si>
+    <t>NBA PRESEASON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCAA FOOTBALLtotal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NHLtotal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NBAtotal </t>
   </si>
 </sst>
 </file>
@@ -412,9 +466,6 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -499,11 +550,214 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -880,935 +1134,1793 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
     <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="29">
+        <v>43010</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="29">
+        <v>43010</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="29">
+        <v>43010</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="8"/>
-      <c r="K2" s="5" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="7"/>
+      <c r="K2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="8" t="e">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="7" t="e">
         <f t="shared" ref="D3:D22" si="0">(C3/B3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="8" t="e">
+      <c r="E3" s="3"/>
+      <c r="F3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="7" t="e">
         <f>(H3/G3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="8" t="e">
+      <c r="K3" s="10"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="7" t="e">
         <f t="shared" ref="N3:N4" si="1">(M3/L3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="8" t="e">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="8" t="e">
+      <c r="E4" s="3"/>
+      <c r="F4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="7" t="e">
         <f t="shared" ref="I4:I13" si="2">(H4/G4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="8" t="e">
+      <c r="K4" s="10"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="7" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="8" t="e">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="8" t="e">
+      <c r="E5" s="3"/>
+      <c r="F5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="8" t="e">
+      <c r="K5" s="10"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="7" t="e">
         <f>(M5/L5)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="8" t="e">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="8" t="e">
+      <c r="E6" s="3"/>
+      <c r="F6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <f>SUM(L3:L5)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <f>SUM(M3:M5)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="8" t="e">
+      <c r="N6" s="7" t="e">
         <f>(M6/L6)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8" t="e">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="8" t="e">
+      <c r="E7" s="3"/>
+      <c r="F7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="8" t="e">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="8" t="e">
+      <c r="E8" s="3"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8" t="e">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="8" t="e">
+      <c r="E9" s="3"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2" t="s">
+      <c r="K9" s="29">
+        <v>43010</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="8" t="e">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="8" t="e">
+      <c r="E10" s="3"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="7"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="8" t="e">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="8" t="e">
+      <c r="E11" s="3"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="8" t="e">
+      <c r="K11" s="10"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="7" t="e">
         <f t="shared" ref="N11:N23" si="3">(M11/L11)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="8" t="e">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="8" t="e">
+      <c r="G12" s="9"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="7" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="8" t="e">
+      <c r="K12" s="10"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="8" t="e">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="15" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="15">
         <f>SUM(G3:G12)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <f>SUM(H3:H12)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="17" t="e">
+      <c r="I13" s="16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="8" t="e">
+      <c r="K13" s="10"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="8" t="e">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="8" t="e">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="8" t="e">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="8" t="e">
+      <c r="E15" s="3"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="8" t="e">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="29">
+        <v>43010</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="8" t="e">
+      <c r="K16" s="10"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="8" t="e">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="8" t="e">
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8" t="e">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="8" t="e">
+      <c r="E18" s="3"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="7" t="e">
         <f t="shared" ref="I18:I28" si="4">(H18/G18)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K18" s="11"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="8" t="e">
+      <c r="K18" s="10"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="8" t="e">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="8" t="e">
+      <c r="E19" s="3"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="7" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="8" t="e">
+      <c r="K19" s="10"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="8" t="e">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="8" t="e">
+      <c r="E20" s="3"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="7" t="e">
         <f>(H20/G20)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="8" t="e">
+      <c r="K20" s="10"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="8" t="e">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="8" t="e">
+      <c r="E21" s="3"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="7" t="e">
         <f>(H21/G21)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="8" t="e">
+      <c r="K21" s="10"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="15">
         <f>SUM(B3:B21)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="15">
         <f>SUM(C3:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="8" t="e">
+      <c r="D22" s="7" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="8" t="e">
+      <c r="E22" s="3"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="7" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="8" t="e">
+      <c r="K22" s="10"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="8" t="e">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="7" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="8" t="e">
+      <c r="L23" s="9">
+        <v>0</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0</v>
+      </c>
+      <c r="N23" s="7" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="29">
+        <v>43010</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" s="9">
+        <f>SUM(L11:L23)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="9">
+        <f>SUM(M11:M23)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="7" t="e">
+        <f>(M24/L24)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="7" t="e">
+        <f>(C26/B26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K26" s="29">
+        <v>43010</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="15">
+        <f>SUM(B26)</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="15">
+        <f>SUM(C26)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="7" t="e">
+        <f>(C27/B27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="3"/>
+      <c r="F28" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="15">
+        <f>SUM(G18:G27)</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="15">
+        <f>SUM(H18:H27)</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="16" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K28" s="10"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="7" t="e">
+        <f t="shared" ref="N28:N40" si="5">(M28/L28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A29" s="29">
+        <v>43010</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D29" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="8" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K24" s="19" t="s">
+      <c r="E29" s="3"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="3"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="27">
+        <f>(B22+G13+L6+B27+G28+L24+L41+G46+L59+L77+G63+L95)</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="27">
+        <f>(C22+C27+H28+H13+M6+M24+M41+H46+M59+M77+H63+M95)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="28" t="e">
+        <f>(C31/B31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="29">
+        <v>43010</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K31" s="10"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F33" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="7" t="e">
+        <f t="shared" ref="I33:I45" si="6">(H33/G33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K33" s="10"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F34" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K34" s="10"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F35" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K35" s="10"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F36" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K36" s="10"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K37" s="10"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F38" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K38" s="10"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F39" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K39" s="10"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F40" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K40" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L40" s="9">
+        <v>0</v>
+      </c>
+      <c r="M40" s="9">
+        <v>0</v>
+      </c>
+      <c r="N40" s="7" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F41" s="10"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K41" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="L24" s="10">
-        <f>SUM(L11:L23)</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="10">
-        <f>SUM(M11:M23)</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="8" t="e">
-        <f>(M24/L24)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="8" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="8" t="e">
-        <f>(C26/B26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="8" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K26" s="1"/>
-      <c r="L26" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M26" s="2" t="s">
+      <c r="L41" s="9">
+        <f>SUM(L28:L40)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="9">
+        <f>SUM(M28:M40)</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="7" t="e">
+        <f>(M41/L41)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F42" s="10"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="10"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F44" s="10"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K44" s="29">
+        <v>43010</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M44" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="N44" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="16">
-        <f>SUM(B26)</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="16">
-        <f>SUM(C26)</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="8" t="e">
-        <f>(C27/B27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="8" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="7"/>
-    </row>
-    <row r="28" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="4"/>
-      <c r="F28" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G28" s="16">
-        <f>SUM(G18:G27)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="16">
-        <f>SUM(H18:H27)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="17" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K28" s="11"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="8" t="e">
-        <f t="shared" ref="N28:N40" si="5">(M28/L28)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="21" t="s">
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G45" s="9">
+        <v>0</v>
+      </c>
+      <c r="H45" s="9">
+        <v>0</v>
+      </c>
+      <c r="I45" s="7" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F46" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G46" s="9">
+        <f>SUM(G33:G45)</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="9">
+        <f>SUM(H33:H45)</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="7" t="e">
+        <f>(H46/G46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K46" s="10"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="7" t="e">
+        <f t="shared" ref="N46:N58" si="7">(M46/L46)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="K47" s="10"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K48" s="10"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F49" s="29"/>
+      <c r="G49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="I49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="4"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="28">
-        <f>(B22+G13+L6+B27+G28+L24+L41)</f>
-        <v>0</v>
-      </c>
-      <c r="C31" s="28">
-        <f>(C22+C27+H28+H13+M6+M24+M41)</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="29" t="e">
-        <f>(C31/B31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K32" s="11"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="33" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K33" s="11"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K34" s="11"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K35" s="11"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K36" s="11"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K37" s="11"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K38" s="11"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K39" s="11"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K40" s="11" t="s">
+      <c r="K49" s="10"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F50" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="6"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F51" s="10"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="7" t="e">
+        <f t="shared" ref="I51:I63" si="8">(H51/G51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K51" s="10"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F52" s="10"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K52" s="10"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F53" s="10"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K53" s="10"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F54" s="10"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K54" s="10"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F55" s="10"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K55" s="10"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F56" s="10"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K56" s="10"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F57" s="10"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K57" s="10"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F58" s="10"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K58" s="10"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="7" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F59" s="10"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K59" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L59" s="9">
+        <f>SUM(L46:L58)</f>
+        <v>0</v>
+      </c>
+      <c r="M59" s="9">
+        <f>SUM(M46:M58)</f>
+        <v>0</v>
+      </c>
+      <c r="N59" s="7" t="e">
+        <f>(M59/L59)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F60" s="10"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="6:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F61" s="10"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F62" s="10"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K62" s="29"/>
+      <c r="L62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N62" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F63" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="7" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="6"/>
+    </row>
+    <row r="64" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F64" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G64" s="9">
+        <f>SUM(G51:G63)</f>
+        <v>0</v>
+      </c>
+      <c r="H64" s="9">
+        <f>SUM(H51:H63)</f>
+        <v>0</v>
+      </c>
+      <c r="I64" s="7" t="e">
+        <f>(H64/G64)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K64" s="10"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="7" t="e">
+        <f t="shared" ref="N64:N76" si="9">(M64/L64)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K65" s="10"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K66" s="10"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K67" s="10"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K68" s="10"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K69" s="10"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K70" s="10"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K71" s="10"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K72" s="10"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K73" s="10"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K74" s="10"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K75" s="10"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K76" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L40" s="10">
-        <v>0</v>
-      </c>
-      <c r="M40" s="10">
-        <v>0</v>
-      </c>
-      <c r="N40" s="8" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K41" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="L41" s="10">
-        <f>SUM(L28:L40)</f>
-        <v>0</v>
-      </c>
-      <c r="M41" s="10">
-        <f>SUM(M28:M40)</f>
-        <v>0</v>
-      </c>
-      <c r="N41" s="8" t="e">
-        <f>(M41/L41)</f>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="7" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K77" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L77" s="9">
+        <f>SUM(L64:L76)</f>
+        <v>0</v>
+      </c>
+      <c r="M77" s="9">
+        <f>SUM(M64:M76)</f>
+        <v>0</v>
+      </c>
+      <c r="N77" s="7" t="e">
+        <f>(M77/L77)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="11:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K80" s="29"/>
+      <c r="L80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K81" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="6"/>
+    </row>
+    <row r="82" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K82" s="10"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="7" t="e">
+        <f t="shared" ref="N82:N94" si="10">(M82/L82)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K83" s="10"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="9"/>
+      <c r="N83" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K84" s="10"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K85" s="10"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K86" s="10"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K87" s="10"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K88" s="10"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K89" s="10"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K90" s="10"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K91" s="10"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K92" s="10"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K93" s="10"/>
+      <c r="L93" s="9"/>
+      <c r="M93" s="9"/>
+      <c r="N93" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K94" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="L94" s="9">
+        <v>0</v>
+      </c>
+      <c r="M94" s="9">
+        <v>0</v>
+      </c>
+      <c r="N94" s="7" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K95" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L95" s="9">
+        <f>SUM(L82:L94)</f>
+        <v>0</v>
+      </c>
+      <c r="M95" s="9">
+        <f>SUM(M82:M94)</f>
+        <v>0</v>
+      </c>
+      <c r="N95" s="7" t="e">
+        <f>(M95/L95)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C31:D31 C26:D27 H3:I13 H18:I28 M3:N6 C3:D22">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:N23">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M24:N24">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M28:N40">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M41:N41">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33:I45">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46:I46">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M46:N58">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M59:N59">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M64:N76">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M77:N77">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1816,7 +2928,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:N23">
+  <conditionalFormatting sqref="M82:N94">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1824,7 +2936,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:N24">
+  <conditionalFormatting sqref="M95:N95">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1832,7 +2944,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M28:N40">
+  <conditionalFormatting sqref="H51:I63">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1840,7 +2952,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M41:N41">
+  <conditionalFormatting sqref="H64:I64">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>